<commit_message>
Add clustering using Kmeans
</commit_message>
<xml_diff>
--- a/data/output/KPIs.xlsx
+++ b/data/output/KPIs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Vie Professionnelle\CDI Dec 2024 - Data Scientist\Entretiens\Quod_Financial\Quod_THA\data\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23458B0B-34F1-4EF6-BA9E-FDA2AA80E16B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ECC3CA6-622C-47A1-A481-0909F6094BBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="yearly" sheetId="1" r:id="rId1"/>
@@ -136,10 +136,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -544,9 +544,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="21.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="12" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -581,7 +592,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
+      <c r="A2" s="3">
         <v>2018</v>
       </c>
       <c r="B2" s="1">
@@ -613,7 +624,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
+      <c r="A3" s="3"/>
       <c r="B3" s="1">
         <v>5</v>
       </c>
@@ -643,7 +654,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="2"/>
+      <c r="A4" s="3"/>
       <c r="B4" s="1">
         <v>6</v>
       </c>
@@ -673,7 +684,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="2"/>
+      <c r="A5" s="3"/>
       <c r="B5" s="1">
         <v>7</v>
       </c>
@@ -703,7 +714,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="2"/>
+      <c r="A6" s="3"/>
       <c r="B6" s="1">
         <v>8</v>
       </c>
@@ -733,7 +744,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="2"/>
+      <c r="A7" s="3"/>
       <c r="B7" s="1">
         <v>9</v>
       </c>
@@ -763,7 +774,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="2"/>
+      <c r="A8" s="3"/>
       <c r="B8" s="1">
         <v>10</v>
       </c>
@@ -793,7 +804,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="2"/>
+      <c r="A9" s="3"/>
       <c r="B9" s="1">
         <v>11</v>
       </c>
@@ -823,7 +834,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="2"/>
+      <c r="A10" s="3"/>
       <c r="B10" s="1">
         <v>12</v>
       </c>
@@ -853,7 +864,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="2">
+      <c r="A11" s="3">
         <v>2019</v>
       </c>
       <c r="B11" s="1">
@@ -885,7 +896,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="2"/>
+      <c r="A12" s="3"/>
       <c r="B12" s="1">
         <v>2</v>
       </c>
@@ -915,7 +926,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="2"/>
+      <c r="A13" s="3"/>
       <c r="B13" s="1">
         <v>3</v>
       </c>
@@ -945,7 +956,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="2"/>
+      <c r="A14" s="3"/>
       <c r="B14" s="1">
         <v>4</v>
       </c>
@@ -975,7 +986,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="2"/>
+      <c r="A15" s="3"/>
       <c r="B15" s="1">
         <v>5</v>
       </c>
@@ -1005,7 +1016,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="2"/>
+      <c r="A16" s="3"/>
       <c r="B16" s="1">
         <v>6</v>
       </c>
@@ -1035,7 +1046,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" s="2"/>
+      <c r="A17" s="3"/>
       <c r="B17" s="1">
         <v>7</v>
       </c>
@@ -1065,7 +1076,7 @@
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" s="2"/>
+      <c r="A18" s="3"/>
       <c r="B18" s="1">
         <v>8</v>
       </c>
@@ -1095,7 +1106,7 @@
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" s="2"/>
+      <c r="A19" s="3"/>
       <c r="B19" s="1">
         <v>9</v>
       </c>
@@ -1137,9 +1148,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -1347,35 +1356,35 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B8" s="3">
+      <c r="B8" s="2">
         <f>AVERAGE(B2:B7)</f>
         <v>112.41543108144447</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="2">
         <f t="shared" ref="C8:I8" si="0">AVERAGE(C2:C7)</f>
         <v>44.4042713595517</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="2">
         <f t="shared" si="0"/>
         <v>102.67933681144478</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="2">
         <f t="shared" si="0"/>
         <v>40.701812761553242</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="2">
         <f t="shared" si="0"/>
         <v>117.97651934902241</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="2">
         <f t="shared" si="0"/>
         <v>52.375212987264</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8" s="2">
         <f t="shared" si="0"/>
         <v>113.75317564268158</v>
       </c>
-      <c r="I8" s="3">
+      <c r="I8" s="2">
         <f t="shared" si="0"/>
         <v>43.514813457758571</v>
       </c>

</xml_diff>

<commit_message>
Add Readme, Docstring and requirements
</commit_message>
<xml_diff>
--- a/data/output/KPIs.xlsx
+++ b/data/output/KPIs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Vie Professionnelle\CDI Dec 2024 - Data Scientist\Entretiens\Quod_Financial\Quod_THA\data\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90B90085-A7D4-48A5-AC7E-0D203AEBB630}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C148CB6-87DD-4C04-9B9B-0F991E745E08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="13">
   <si>
     <t>year</t>
   </si>
@@ -50,6 +50,18 @@
   </si>
   <si>
     <t>KNeighborsRegressor_MAE</t>
+  </si>
+  <si>
+    <t>RandomForest_RMSE</t>
+  </si>
+  <si>
+    <t>RandomForest_MAE</t>
+  </si>
+  <si>
+    <t>XGBoost_RMSE</t>
+  </si>
+  <si>
+    <t>XGBoost_MAE</t>
   </si>
   <si>
     <t>MLP_RMSE</t>
@@ -436,13 +448,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -464,50 +476,86 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>2018</v>
       </c>
       <c r="B2">
-        <v>126.3887594168869</v>
+        <v>156.52367005301491</v>
       </c>
       <c r="C2">
-        <v>63.059986505675511</v>
+        <v>73.717485972118283</v>
       </c>
       <c r="D2">
-        <v>170.38103395395839</v>
+        <v>169.22741686281969</v>
       </c>
       <c r="E2">
-        <v>67.879684223510537</v>
+        <v>66.332297472989254</v>
       </c>
       <c r="F2">
+        <v>154.2681548989847</v>
+      </c>
+      <c r="G2">
+        <v>60.459443345487841</v>
+      </c>
+      <c r="H2">
+        <v>170.28000263352999</v>
+      </c>
+      <c r="I2">
+        <v>70.114959716796875</v>
+      </c>
+      <c r="J2">
         <v>192.5173633065867</v>
       </c>
-      <c r="G2">
+      <c r="K2">
         <v>68.642785585153916</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2019</v>
       </c>
       <c r="B3">
-        <v>99.325195644291185</v>
+        <v>116.0262056294069</v>
       </c>
       <c r="C3">
-        <v>50.105059765965322</v>
+        <v>56.547561306853858</v>
       </c>
       <c r="D3">
-        <v>110.7254787741274</v>
+        <v>104.3126050507923</v>
       </c>
       <c r="E3">
-        <v>46.437533368926857</v>
+        <v>43.999884721667193</v>
       </c>
       <c r="F3">
+        <v>105.43469278014121</v>
+      </c>
+      <c r="G3">
+        <v>42.205817227074348</v>
+      </c>
+      <c r="H3">
+        <v>133.71595653193381</v>
+      </c>
+      <c r="I3">
+        <v>51.258819580078118</v>
+      </c>
+      <c r="J3">
         <v>113.8506388186275</v>
       </c>
-      <c r="G3">
+      <c r="K3">
         <v>49.06485462590436</v>
       </c>
     </row>
@@ -518,18 +566,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -549,8 +597,20 @@
       <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>2018</v>
       </c>
@@ -558,217 +618,325 @@
         <v>4</v>
       </c>
       <c r="C2">
-        <v>143.6365031322425</v>
+        <v>161.31912114858079</v>
       </c>
       <c r="D2">
-        <v>80.609929391206563</v>
+        <v>81.198257768093015</v>
       </c>
       <c r="E2">
-        <v>178.8953103928018</v>
+        <v>173.07922243972999</v>
       </c>
       <c r="F2">
-        <v>76.574944071588362</v>
+        <v>73.818677805130747</v>
       </c>
       <c r="G2">
+        <v>155.77814430408901</v>
+      </c>
+      <c r="H2">
+        <v>60.14513126199558</v>
+      </c>
+      <c r="I2">
+        <v>167.59280311591539</v>
+      </c>
+      <c r="J2">
+        <v>70.611503601074219</v>
+      </c>
+      <c r="K2">
         <v>210.47726174783801</v>
       </c>
-      <c r="H2">
+      <c r="L2">
         <v>75.755881758228412</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="1">
         <v>5</v>
       </c>
       <c r="C3">
-        <v>131.67944511655469</v>
+        <v>173.40260948165991</v>
       </c>
       <c r="D3">
-        <v>79.591796505737605</v>
+        <v>81.130775549380473</v>
       </c>
       <c r="E3">
-        <v>190.43634905920379</v>
+        <v>192.63220646502569</v>
       </c>
       <c r="F3">
-        <v>74.110474090407934</v>
+        <v>72.717838092272203</v>
       </c>
       <c r="G3">
+        <v>167.93377838148609</v>
+      </c>
+      <c r="H3">
+        <v>59.223353209796507</v>
+      </c>
+      <c r="I3">
+        <v>184.2310348957254</v>
+      </c>
+      <c r="J3">
+        <v>70.175865173339844</v>
+      </c>
+      <c r="K3">
         <v>202.76353616319929</v>
       </c>
-      <c r="H3">
+      <c r="L3">
         <v>76.591916609087477</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="B4" s="1">
         <v>6</v>
       </c>
       <c r="C4">
-        <v>113.9231716567741</v>
+        <v>151.79717287317561</v>
       </c>
       <c r="D4">
-        <v>68.091400609841358</v>
+        <v>74.873450568256899</v>
       </c>
       <c r="E4">
-        <v>167.95847026030401</v>
+        <v>175.92118874030399</v>
       </c>
       <c r="F4">
-        <v>59.806263498920103</v>
+        <v>58.742235968255571</v>
       </c>
       <c r="G4">
+        <v>147.2995759864605</v>
+      </c>
+      <c r="H4">
+        <v>60.621986522873648</v>
+      </c>
+      <c r="I4">
+        <v>163.7527015521423</v>
+      </c>
+      <c r="J4">
+        <v>67.178024291992188</v>
+      </c>
+      <c r="K4">
         <v>193.35333568397871</v>
       </c>
-      <c r="H4">
+      <c r="L4">
         <v>73.607651269520119</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="B5" s="1">
         <v>7</v>
       </c>
       <c r="C5">
-        <v>133.0694862906164</v>
+        <v>172.77492253852159</v>
       </c>
       <c r="D5">
-        <v>61.374722777833881</v>
+        <v>72.992310651974137</v>
       </c>
       <c r="E5">
-        <v>175.80372124757309</v>
+        <v>173.58889766740469</v>
       </c>
       <c r="F5">
-        <v>65.088988764044942</v>
+        <v>63.636917191188083</v>
       </c>
       <c r="G5">
+        <v>168.76141235299201</v>
+      </c>
+      <c r="H5">
+        <v>64.288474351701197</v>
+      </c>
+      <c r="I5">
+        <v>180.80087674358771</v>
+      </c>
+      <c r="J5">
+        <v>69.194099426269531</v>
+      </c>
+      <c r="K5">
         <v>175.4396583451101</v>
       </c>
-      <c r="H5">
+      <c r="L5">
         <v>65.736536374296335</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" s="1">
         <v>8</v>
       </c>
       <c r="C6">
-        <v>153.5146927489003</v>
+        <v>189.5309205992445</v>
       </c>
       <c r="D6">
-        <v>63.685951956026408</v>
+        <v>79.469600280957479</v>
       </c>
       <c r="E6">
-        <v>185.10002993268549</v>
+        <v>190.24385636764919</v>
       </c>
       <c r="F6">
-        <v>75.363063063063052</v>
+        <v>74.932448750178708</v>
       </c>
       <c r="G6">
+        <v>185.72530693134451</v>
+      </c>
+      <c r="H6">
+        <v>65.647336210019631</v>
+      </c>
+      <c r="I6">
+        <v>200.2761179908878</v>
+      </c>
+      <c r="J6">
+        <v>74.986923217773438</v>
+      </c>
+      <c r="K6">
         <v>152.0103710881688</v>
       </c>
-      <c r="H6">
+      <c r="L6">
         <v>63.621972119212998</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="1">
         <v>9</v>
       </c>
       <c r="C7">
-        <v>137.25295738142961</v>
+        <v>183.8967028575</v>
       </c>
       <c r="D7">
-        <v>65.150147853291614</v>
+        <v>85.492144389705615</v>
       </c>
       <c r="E7">
-        <v>211.10637865801721</v>
+        <v>207.0844366902592</v>
       </c>
       <c r="F7">
-        <v>87.972304199772992</v>
+        <v>85.962453355320633</v>
       </c>
       <c r="G7">
+        <v>159.93225514626371</v>
+      </c>
+      <c r="H7">
+        <v>69.529376563813315</v>
+      </c>
+      <c r="I7">
+        <v>189.05132198360849</v>
+      </c>
+      <c r="J7">
+        <v>81.791023254394531</v>
+      </c>
+      <c r="K7">
         <v>207.92559743844629</v>
       </c>
-      <c r="H7">
+      <c r="L7">
         <v>78.32595362482428</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="B8" s="1">
         <v>10</v>
       </c>
       <c r="C8">
-        <v>121.2281019882986</v>
+        <v>137.5177804102361</v>
       </c>
       <c r="D8">
-        <v>56.270755886160913</v>
+        <v>69.908649976805137</v>
       </c>
       <c r="E8">
-        <v>152.74924453224151</v>
+        <v>150.51399656229381</v>
       </c>
       <c r="F8">
-        <v>65.942354235423551</v>
+        <v>64.244803427677283</v>
       </c>
       <c r="G8">
+        <v>180.0839217584433</v>
+      </c>
+      <c r="H8">
+        <v>65.876328546293536</v>
+      </c>
+      <c r="I8">
+        <v>171.30803076986791</v>
+      </c>
+      <c r="J8">
+        <v>75.253829956054688</v>
+      </c>
+      <c r="K8">
         <v>230.6171320669188</v>
       </c>
-      <c r="H8">
+      <c r="L8">
         <v>71.581368529085609</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="1">
         <v>11</v>
       </c>
       <c r="C9">
-        <v>104.384819759642</v>
+        <v>115.2175207623537</v>
       </c>
       <c r="D9">
-        <v>48.603488400183771</v>
+        <v>64.027673667440283</v>
       </c>
       <c r="E9">
-        <v>136.17001703187651</v>
+        <v>124.8634506714973</v>
       </c>
       <c r="F9">
-        <v>58.256043956043953</v>
+        <v>56.614652190844168</v>
       </c>
       <c r="G9">
+        <v>111.41874859255201</v>
+      </c>
+      <c r="H9">
+        <v>54.66055904505739</v>
+      </c>
+      <c r="I9">
+        <v>133.43537029916391</v>
+      </c>
+      <c r="J9">
+        <v>66.439125061035156</v>
+      </c>
+      <c r="K9">
         <v>217.38895750406431</v>
       </c>
-      <c r="H9">
+      <c r="L9">
         <v>65.700945225393667</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="1">
         <v>12</v>
       </c>
       <c r="C10">
-        <v>86.536574275131485</v>
+        <v>101.0675219850619</v>
       </c>
       <c r="D10">
-        <v>44.308688378818843</v>
+        <v>54.828271705575872</v>
       </c>
       <c r="E10">
-        <v>117.43681076767029</v>
+        <v>113.1747613538537</v>
       </c>
       <c r="F10">
-        <v>48.707317073170742</v>
+        <v>47.210638573903609</v>
       </c>
       <c r="G10">
+        <v>83.454196096654655</v>
+      </c>
+      <c r="H10">
+        <v>44.494201898409443</v>
+      </c>
+      <c r="I10">
+        <v>130.07922015304749</v>
+      </c>
+      <c r="J10">
+        <v>55.814357757568359</v>
+      </c>
+      <c r="K10">
         <v>113.431670147239</v>
       </c>
-      <c r="H10">
+      <c r="L10">
         <v>46.861899224463848</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>2019</v>
       </c>
@@ -776,213 +944,321 @@
         <v>1</v>
       </c>
       <c r="C11">
-        <v>108.746469626652</v>
+        <v>94.907148429272709</v>
       </c>
       <c r="D11">
-        <v>65.794100161914997</v>
+        <v>57.177754232343872</v>
       </c>
       <c r="E11">
-        <v>108.3024420194135</v>
+        <v>93.554754629353909</v>
       </c>
       <c r="F11">
-        <v>50.133034714445692</v>
+        <v>45.841109919985271</v>
       </c>
       <c r="G11">
+        <v>111.1594989781828</v>
+      </c>
+      <c r="H11">
+        <v>53.364736880175691</v>
+      </c>
+      <c r="I11">
+        <v>120.8340642937661</v>
+      </c>
+      <c r="J11">
+        <v>56.510051727294922</v>
+      </c>
+      <c r="K11">
         <v>149.29746776051951</v>
       </c>
-      <c r="H11">
+      <c r="L11">
         <v>64.499885382577432</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="1">
         <v>2</v>
       </c>
       <c r="C12">
-        <v>100.5693114250857</v>
+        <v>115.1614386917969</v>
       </c>
       <c r="D12">
-        <v>52.485951934605779</v>
+        <v>56.906788745001442</v>
       </c>
       <c r="E12">
-        <v>109.3020239677149</v>
+        <v>106.1042845181113</v>
       </c>
       <c r="F12">
-        <v>47.008823529411771</v>
+        <v>45.444933317158522</v>
       </c>
       <c r="G12">
+        <v>115.7395708278442</v>
+      </c>
+      <c r="H12">
+        <v>42.147438282183991</v>
+      </c>
+      <c r="I12">
+        <v>140.84209631267919</v>
+      </c>
+      <c r="J12">
+        <v>52.069477081298828</v>
+      </c>
+      <c r="K12">
         <v>100.6285405313758</v>
       </c>
-      <c r="H12">
+      <c r="L12">
         <v>44.452975019540311</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="1">
         <v>3</v>
       </c>
       <c r="C13">
-        <v>96.47427434760381</v>
+        <v>115.02086386918</v>
       </c>
       <c r="D13">
-        <v>55.102173732385658</v>
+        <v>60.829947166389509</v>
       </c>
       <c r="E13">
-        <v>98.974983272389366</v>
+        <v>100.5091048137546</v>
       </c>
       <c r="F13">
-        <v>47.497968397291203</v>
+        <v>47.606849188495872</v>
       </c>
       <c r="G13">
+        <v>113.6376969496651</v>
+      </c>
+      <c r="H13">
+        <v>45.612635939444857</v>
+      </c>
+      <c r="I13">
+        <v>141.48027413300409</v>
+      </c>
+      <c r="J13">
+        <v>55.351535797119141</v>
+      </c>
+      <c r="K13">
         <v>102.6804891141668</v>
       </c>
-      <c r="H13">
+      <c r="L13">
         <v>51.605298774603042</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
       <c r="B14" s="1">
         <v>4</v>
       </c>
       <c r="C14">
-        <v>110.7031370243017</v>
+        <v>137.3372865546844</v>
       </c>
       <c r="D14">
-        <v>52.054519666092453</v>
+        <v>60.338809718930086</v>
       </c>
       <c r="E14">
-        <v>116.7965607188186</v>
+        <v>114.15603530097739</v>
       </c>
       <c r="F14">
-        <v>50.169739952718693</v>
+        <v>48.378831264701162</v>
       </c>
       <c r="G14">
+        <v>112.61695531024959</v>
+      </c>
+      <c r="H14">
+        <v>44.195155461488717</v>
+      </c>
+      <c r="I14">
+        <v>148.1067565242214</v>
+      </c>
+      <c r="J14">
+        <v>53.455661773681641</v>
+      </c>
+      <c r="K14">
         <v>119.5119213278615</v>
       </c>
-      <c r="H14">
+      <c r="L14">
         <v>50.005086336518573</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
       <c r="B15" s="1">
         <v>5</v>
       </c>
       <c r="C15">
-        <v>106.82978485260961</v>
+        <v>141.8838933305355</v>
       </c>
       <c r="D15">
-        <v>50.773636634015467</v>
+        <v>61.609280922315158</v>
       </c>
       <c r="E15">
-        <v>112.52556616333931</v>
+        <v>109.8864493395742</v>
       </c>
       <c r="F15">
-        <v>48.245130641330171</v>
+        <v>46.223918425947581</v>
       </c>
       <c r="G15">
+        <v>110.8690343362119</v>
+      </c>
+      <c r="H15">
+        <v>47.215045104498223</v>
+      </c>
+      <c r="I15">
+        <v>150.58781309629609</v>
+      </c>
+      <c r="J15">
+        <v>56.109603881835938</v>
+      </c>
+      <c r="K15">
         <v>111.15011968713451</v>
       </c>
-      <c r="H15">
+      <c r="L15">
         <v>48.974253423352387</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
       <c r="B16" s="1">
         <v>6</v>
       </c>
       <c r="C16">
-        <v>90.566157284178772</v>
+        <v>125.6666502822947</v>
       </c>
       <c r="D16">
-        <v>43.806000740015797</v>
+        <v>58.131176009203116</v>
       </c>
       <c r="E16">
-        <v>109.1074723670005</v>
+        <v>98.239770857989512</v>
       </c>
       <c r="F16">
-        <v>42.279665071770339</v>
+        <v>39.377563389493197</v>
       </c>
       <c r="G16">
+        <v>94.57080990833721</v>
+      </c>
+      <c r="H16">
+        <v>36.614226996045851</v>
+      </c>
+      <c r="I16">
+        <v>131.25161457340249</v>
+      </c>
+      <c r="J16">
+        <v>49.209938049316413</v>
+      </c>
+      <c r="K16">
         <v>117.43903948086199</v>
       </c>
-      <c r="H16">
+      <c r="L16">
         <v>45.675845799899761</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
       <c r="B17" s="1">
         <v>7</v>
       </c>
       <c r="C17">
-        <v>94.57185748508337</v>
+        <v>108.7597354114627</v>
       </c>
       <c r="D17">
-        <v>42.75073140473225</v>
+        <v>51.13001185988653</v>
       </c>
       <c r="E17">
-        <v>118.7755609417985</v>
+        <v>108.2934599669307</v>
       </c>
       <c r="F17">
-        <v>43.067754077791719</v>
+        <v>39.253238933257563</v>
       </c>
       <c r="G17">
+        <v>97.270048143097071</v>
+      </c>
+      <c r="H17">
+        <v>36.633436320800691</v>
+      </c>
+      <c r="I17">
+        <v>127.63517267856651</v>
+      </c>
+      <c r="J17">
+        <v>47.023452758789063</v>
+      </c>
+      <c r="K17">
         <v>106.6236865570407</v>
       </c>
-      <c r="H17">
+      <c r="L17">
         <v>46.165949432608308</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
       <c r="B18" s="1">
         <v>8</v>
       </c>
       <c r="C18">
-        <v>89.785336300380067</v>
+        <v>92.386558821582781</v>
       </c>
       <c r="D18">
-        <v>41.282499000339733</v>
+        <v>49.989998539072118</v>
       </c>
       <c r="E18">
-        <v>117.9514673620034</v>
+        <v>107.68719285629869</v>
       </c>
       <c r="F18">
-        <v>43.730829015544039</v>
+        <v>40.913916160009798</v>
       </c>
       <c r="G18">
+        <v>87.75323217210331</v>
+      </c>
+      <c r="H18">
+        <v>35.658334163274738</v>
+      </c>
+      <c r="I18">
+        <v>112.4236589938368</v>
+      </c>
+      <c r="J18">
+        <v>44.405014038085938</v>
+      </c>
+      <c r="K18">
         <v>101.1473642069431</v>
       </c>
-      <c r="H18">
+      <c r="L18">
         <v>43.139702245709337</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
       <c r="B19" s="1">
         <v>9</v>
       </c>
       <c r="C19">
-        <v>90.12860504992193</v>
+        <v>99.201270967389391</v>
       </c>
       <c r="D19">
-        <v>43.561283186269819</v>
+        <v>50.993819720750572</v>
       </c>
       <c r="E19">
-        <v>104.2552719968177</v>
+        <v>99.203640869024753</v>
       </c>
       <c r="F19">
-        <v>44.84402173913044</v>
+        <v>41.737754727273177</v>
       </c>
       <c r="G19">
+        <v>97.002375249689777</v>
+      </c>
+      <c r="H19">
+        <v>35.871461628556787</v>
+      </c>
+      <c r="I19">
+        <v>121.43659932759149</v>
+      </c>
+      <c r="J19">
+        <v>45.015026092529297</v>
+      </c>
+      <c r="K19">
         <v>103.8566115276451</v>
       </c>
-      <c r="H19">
+      <c r="L19">
         <v>45.044871244173692</v>
       </c>
     </row>
@@ -997,17 +1273,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1027,167 +1303,267 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>130.14546836096861</v>
+        <v>162.3474127638753</v>
       </c>
       <c r="C2">
-        <v>76.020415574314541</v>
+        <v>79.028115546083271</v>
       </c>
       <c r="D2">
-        <v>179.257040056937</v>
+        <v>180.75274551576891</v>
       </c>
       <c r="E2">
-        <v>70.061166116611673</v>
+        <v>68.333072099040137</v>
       </c>
       <c r="F2">
+        <v>157.1719164991475</v>
+      </c>
+      <c r="G2">
+        <v>60.000472398126327</v>
+      </c>
+      <c r="H2">
+        <v>172.05298738688029</v>
+      </c>
+      <c r="I2">
+        <v>69.300712585449219</v>
+      </c>
+      <c r="J2">
         <v>202.21846988308579</v>
       </c>
-      <c r="G2">
+      <c r="K2">
         <v>75.304478082828808</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>141.5589821866055</v>
+        <v>182.18917552891381</v>
       </c>
       <c r="C3">
-        <v>63.397483590813671</v>
+        <v>79.297006670582135</v>
       </c>
       <c r="D3">
-        <v>191.18838133324391</v>
+        <v>190.73931862322581</v>
       </c>
       <c r="E3">
-        <v>76.101993230537801</v>
+        <v>74.806240013671896</v>
       </c>
       <c r="F3">
+        <v>171.83461106554091</v>
+      </c>
+      <c r="G3">
+        <v>66.478735419417461</v>
+      </c>
+      <c r="H3">
+        <v>190.20645649859</v>
+      </c>
+      <c r="I3">
+        <v>75.302383422851563</v>
+      </c>
+      <c r="J3">
         <v>179.84244497973921</v>
       </c>
-      <c r="G3">
+      <c r="K3">
         <v>69.201577193852984</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>105.0526637385142</v>
+        <v>118.9259715508949</v>
       </c>
       <c r="C4">
-        <v>49.741171798008857</v>
+        <v>62.942758891847113</v>
       </c>
       <c r="D4">
-        <v>136.26293480506919</v>
+        <v>130.49238166171921</v>
       </c>
       <c r="E4">
-        <v>57.658434399117972</v>
+        <v>56.046253510873903</v>
       </c>
       <c r="F4">
+        <v>131.508095682494</v>
+      </c>
+      <c r="G4">
+        <v>55.037288310161117</v>
+      </c>
+      <c r="H4">
+        <v>146.17611648709919</v>
+      </c>
+      <c r="I4">
+        <v>65.861778259277344</v>
+      </c>
+      <c r="J4">
         <v>194.51788255130759</v>
       </c>
-      <c r="G4">
+      <c r="K4">
         <v>61.420344450023322</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>102.0768754086094</v>
+        <v>108.7410069431822</v>
       </c>
       <c r="C5">
-        <v>57.819090830520203</v>
+        <v>58.302917374947597</v>
       </c>
       <c r="D5">
-        <v>105.6332180852652</v>
+        <v>100.1662077959782</v>
       </c>
       <c r="E5">
-        <v>48.219226436349977</v>
+        <v>46.297071194863811</v>
       </c>
       <c r="F5">
+        <v>113.5198514072021</v>
+      </c>
+      <c r="G5">
+        <v>47.061900457302173</v>
+      </c>
+      <c r="H5">
+        <v>134.68757975635691</v>
+      </c>
+      <c r="I5">
+        <v>54.650524139404297</v>
+      </c>
+      <c r="J5">
         <v>119.7656306811699</v>
       </c>
-      <c r="G5">
+      <c r="K5">
         <v>53.555059060538333</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6">
-        <v>103.1100398260599</v>
+        <v>135.16057108106131</v>
       </c>
       <c r="C6">
-        <v>48.895143542792567</v>
+        <v>60.03142262381062</v>
       </c>
       <c r="D6">
-        <v>112.8688252422649</v>
+        <v>107.6697984954359</v>
       </c>
       <c r="E6">
-        <v>46.914342313787643</v>
+        <v>44.678555292472787</v>
       </c>
       <c r="F6">
+        <v>106.36658565368189</v>
+      </c>
+      <c r="G6">
+        <v>42.691625700119367</v>
+      </c>
+      <c r="H6">
+        <v>143.607946115457</v>
+      </c>
+      <c r="I6">
+        <v>52.934738159179688</v>
+      </c>
+      <c r="J6">
         <v>116.0904269924753</v>
       </c>
-      <c r="G6">
+      <c r="K6">
         <v>48.227270805021249</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7">
-        <v>91.576439747332415</v>
+        <v>100.4536087094986</v>
       </c>
       <c r="C7">
-        <v>42.517798951378943</v>
+        <v>50.704707001720458</v>
       </c>
       <c r="D7">
-        <v>114.0536365810121</v>
+        <v>105.26809360014229</v>
       </c>
       <c r="E7">
-        <v>43.857006507592189</v>
+        <v>40.602760166857657</v>
       </c>
       <c r="F7">
+        <v>94.101608326830458</v>
+      </c>
+      <c r="G7">
+        <v>36.063548147654679</v>
+      </c>
+      <c r="H7">
+        <v>120.7258726542285</v>
+      </c>
+      <c r="I7">
+        <v>45.505172729492188</v>
+      </c>
+      <c r="J7">
         <v>103.93054581187501</v>
       </c>
-      <c r="G7">
+      <c r="K7">
         <v>44.7944195519255</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B8" s="3">
         <f>AVERAGE(B2:B7)</f>
-        <v>112.25341154468167</v>
+        <v>134.6362910962377</v>
       </c>
       <c r="C8" s="3">
-        <f t="shared" ref="C8:G8" si="0">AVERAGE(C2:C7)</f>
-        <v>56.398517381304792</v>
+        <f t="shared" ref="C8:K8" si="0">AVERAGE(C2:C7)</f>
+        <v>65.051154684831872</v>
       </c>
       <c r="D8" s="3">
         <f t="shared" si="0"/>
-        <v>139.87733935063204</v>
+        <v>135.8480909487117</v>
       </c>
       <c r="E8" s="3">
         <f t="shared" si="0"/>
-        <v>57.1353615006662</v>
+        <v>55.12732537963003</v>
       </c>
       <c r="F8" s="3">
         <f t="shared" si="0"/>
+        <v>129.08377810581615</v>
+      </c>
+      <c r="G8" s="3">
+        <f t="shared" si="0"/>
+        <v>51.222261738796846</v>
+      </c>
+      <c r="H8" s="3">
+        <f t="shared" si="0"/>
+        <v>151.24282648310199</v>
+      </c>
+      <c r="I8" s="3">
+        <f t="shared" si="0"/>
+        <v>60.592551549275719</v>
+      </c>
+      <c r="J8" s="3">
+        <f t="shared" si="0"/>
         <v>152.7275668166088</v>
       </c>
-      <c r="G8" s="3">
+      <c r="K8" s="3">
         <f t="shared" si="0"/>
         <v>58.750524857365036</v>
       </c>

</xml_diff>